<commit_message>
"Deleted entire frontend codebase, including API config, data API, types, and dependencies."
</commit_message>
<xml_diff>
--- a/data/Расчет маршрутов прямоточники 11 кр.xlsx
+++ b/data/Расчет маршрутов прямоточники 11 кр.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma.toshkin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Projects\pathfinder\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA124DD-3BF5-4C76-9A40-3094D942FD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="15450" windowHeight="11385"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="расчет" sheetId="1" r:id="rId1"/>
@@ -89,7 +90,18 @@
     <definedName name="wvu.BSTHEOR." localSheetId="0" hidden="1">{TRUE,TRUE,-1.25,-15.5,484.5,279.75,FALSE,FALSE,TRUE,TRUE,0,1,#N/A,1,#N/A,11.171875,17.8235294117647,1,FALSE,FALSE,3,TRUE,1,FALSE,100,"Swvu.BSTHEOR.","ACwvu.BSTHEOR.",1,FALSE,FALSE,0.75,0.75,1,1,1,"","",FALSE,FALSE,FALSE,FALSE,1,100,#N/A,#N/A,"=R1C1:R43C11",FALSE,#N/A,#N/A,FALSE,FALSE}</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">расчет!$A$1:$O$126</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -443,7 +455,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;&quot;-&quot;&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.00&quot; mm dia&quot;"/>
@@ -1298,6 +1310,30 @@
     </xf>
     <xf numFmtId="170" fontId="23" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1319,15 +1355,6 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1343,24 +1370,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal_NEW  B &amp; S  MACHINE" xfId="2"/>
+    <cellStyle name="Normal_NEW  B &amp; S  MACHINE" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1553,7 +1565,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1611,7 +1629,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1651,6 +1675,13 @@
           </a:ext>
         </a:extLst>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1733,6 +1764,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1768,6 +1816,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1943,12 +2008,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:W123"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2290,7 +2355,7 @@
       <c r="N15" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="O15" s="149" t="s">
+      <c r="O15" s="157" t="s">
         <v>91</v>
       </c>
       <c r="P15" s="24"/>
@@ -2339,14 +2404,14 @@
       <c r="N16" s="58">
         <v>11</v>
       </c>
-      <c r="O16" s="149"/>
+      <c r="O16" s="157"/>
     </row>
     <row r="17" spans="1:23" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="153" t="s">
+      <c r="A17" s="161" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="154"/>
-      <c r="C17" s="155"/>
+      <c r="B17" s="162"/>
+      <c r="C17" s="163"/>
       <c r="D17" s="60">
         <f t="shared" ref="D17:K17" si="0">(INSIZE^2-D19^2)/(INSIZE^2)</f>
         <v>0.24202806024519563</v>
@@ -2402,11 +2467,11 @@
       <c r="W17" s="24"/>
     </row>
     <row r="18" spans="1:23" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="156" t="s">
+      <c r="A18" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="157"/>
-      <c r="C18" s="158"/>
+      <c r="B18" s="152"/>
+      <c r="C18" s="153"/>
       <c r="D18" s="61">
         <f>IF(D$16&lt;STRTBLK,"OMIT",IF(E6&gt;0,E6,(TAPER*($L$2-D$16)/100+AVREDN)))</f>
         <v>0.2420280602451956</v>
@@ -2647,7 +2712,7 @@
         <v>2342.305979474535</v>
       </c>
     </row>
-    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="63" t="s">
         <v>25</v>
       </c>
@@ -2692,7 +2757,7 @@
       <c r="M22" s="71"/>
       <c r="N22" s="24"/>
     </row>
-    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="72"/>
       <c r="B23" s="72"/>
       <c r="C23" s="72"/>
@@ -2708,7 +2773,7 @@
       <c r="M23" s="71"/>
       <c r="N23" s="24"/>
     </row>
-    <row r="24" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A24" s="72" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2818,7 @@
       <c r="M24" s="71"/>
       <c r="N24" s="24"/>
     </row>
-    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="72"/>
       <c r="B25" s="72"/>
       <c r="C25" s="72"/>
@@ -2778,7 +2843,7 @@
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="72" t="s">
         <v>27</v>
       </c>
@@ -2825,7 +2890,7 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="72" t="s">
         <v>28</v>
       </c>
@@ -2880,7 +2945,7 @@
       <c r="V27" s="24"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A28" s="72" t="s">
         <v>29</v>
       </c>
@@ -2925,7 +2990,7 @@
       <c r="M28" s="71"/>
       <c r="N28" s="24"/>
     </row>
-    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="72" t="s">
         <v>30</v>
       </c>
@@ -2970,7 +3035,7 @@
       <c r="M29" s="71"/>
       <c r="N29" s="24"/>
     </row>
-    <row r="30" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A30" s="72" t="s">
         <v>31</v>
       </c>
@@ -3014,7 +3079,7 @@
       </c>
       <c r="M30" s="71"/>
     </row>
-    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="72" t="s">
         <v>32</v>
       </c>
@@ -3062,7 +3127,7 @@
       </c>
       <c r="R31" s="24"/>
     </row>
-    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="72" t="s">
         <v>33</v>
       </c>
@@ -3107,7 +3172,7 @@
       <c r="M32" s="71"/>
       <c r="N32" s="24"/>
     </row>
-    <row r="33" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A33" s="72" t="s">
         <v>34</v>
       </c>
@@ -3155,7 +3220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A34" s="72" t="s">
         <v>35</v>
       </c>
@@ -3203,7 +3268,7 @@
       </c>
       <c r="N34" s="24"/>
     </row>
-    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="72" t="s">
         <v>36</v>
       </c>
@@ -3256,7 +3321,7 @@
       <c r="V35" s="24"/>
       <c r="W35" s="24"/>
     </row>
-    <row r="36" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A36" s="72" t="s">
         <v>37</v>
       </c>
@@ -3310,7 +3375,7 @@
       <c r="V36" s="24"/>
       <c r="W36" s="24"/>
     </row>
-    <row r="37" spans="1:23" ht="21.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A37" s="86" t="s">
         <v>38</v>
       </c>
@@ -3363,7 +3428,7 @@
       <c r="V37" s="24"/>
       <c r="W37" s="24"/>
     </row>
-    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="89"/>
       <c r="B38" s="90"/>
       <c r="C38" s="90"/>
@@ -3388,7 +3453,7 @@
       <c r="V38" s="24"/>
       <c r="W38" s="24"/>
     </row>
-    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="N39" s="24"/>
       <c r="O39" s="24"/>
       <c r="P39" s="24"/>
@@ -3400,7 +3465,7 @@
       <c r="V39" s="24"/>
       <c r="W39" s="24"/>
     </row>
-    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>39</v>
       </c>
@@ -3418,7 +3483,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G41" s="16" t="s">
         <v>41</v>
       </c>
@@ -3829,11 +3894,11 @@
       <c r="W60" s="24"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A61" s="159" t="s">
+      <c r="A61" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="160"/>
-      <c r="C61" s="161"/>
+      <c r="B61" s="165"/>
+      <c r="C61" s="166"/>
       <c r="D61" s="119">
         <f t="shared" ref="D61:M61" si="13">($E$51^2-D63^2)/$E$51^2</f>
         <v>0.66761245314452322</v>
@@ -3886,11 +3951,11 @@
       <c r="W61" s="24"/>
     </row>
     <row r="62" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="162" t="s">
+      <c r="A62" s="167" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="162"/>
-      <c r="C62" s="162"/>
+      <c r="B62" s="167"/>
+      <c r="C62" s="167"/>
       <c r="D62" s="120">
         <f>IF(D63="OMIT",D63,1-(D63/INSIZE)^2)</f>
         <v>-0.99515625000000019</v>
@@ -3943,11 +4008,11 @@
       <c r="W62" s="24"/>
     </row>
     <row r="63" spans="1:23" ht="12.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="163" t="s">
+      <c r="A63" s="168" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="163"/>
-      <c r="C63" s="163"/>
+      <c r="B63" s="168"/>
+      <c r="C63" s="168"/>
       <c r="D63" s="123">
         <v>5.65</v>
       </c>
@@ -3976,11 +4041,11 @@
       <c r="M63" s="126"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A64" s="150" t="s">
+      <c r="A64" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B64" s="151"/>
-      <c r="C64" s="152"/>
+      <c r="B64" s="159"/>
+      <c r="C64" s="160"/>
       <c r="D64" s="67">
         <f>SUM(D13+(SUM(0.6*($D$12+(INSIZE/40)+D62)*(D$17*100))/(SUM((LOG(100-D$17*100))/2)+0.0005*D$17*100)))</f>
         <v>127.78563797898765</v>
@@ -4067,7 +4132,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="127" t="s">
         <v>56</v>
       </c>
@@ -4111,7 +4176,7 @@
       </c>
       <c r="M66" s="118"/>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="127"/>
       <c r="B67" s="127"/>
       <c r="C67" s="127"/>
@@ -4126,7 +4191,7 @@
       <c r="L67" s="130"/>
       <c r="M67" s="118"/>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="127" t="s">
         <v>57</v>
       </c>
@@ -4169,7 +4234,7 @@
       </c>
       <c r="M68" s="118"/>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="127"/>
       <c r="B69" s="127"/>
       <c r="C69" s="127"/>
@@ -4184,7 +4249,7 @@
       <c r="L69" s="130"/>
       <c r="M69" s="118"/>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="127" t="s">
         <v>58</v>
       </c>
@@ -4227,7 +4292,7 @@
       </c>
       <c r="M70" s="118"/>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="127" t="s">
         <v>59</v>
       </c>
@@ -4270,7 +4335,7 @@
       </c>
       <c r="M71" s="118"/>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="127"/>
       <c r="B72" s="127"/>
       <c r="C72" s="127"/>
@@ -4285,7 +4350,7 @@
       <c r="L72" s="132"/>
       <c r="M72" s="118"/>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="127" t="s">
         <v>60</v>
       </c>
@@ -4329,7 +4394,7 @@
       </c>
       <c r="M73" s="118"/>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="127" t="s">
         <v>61</v>
       </c>
@@ -4373,7 +4438,7 @@
       </c>
       <c r="M74" s="118"/>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="127"/>
       <c r="B75" s="127"/>
       <c r="C75" s="127"/>
@@ -4388,7 +4453,7 @@
       <c r="L75" s="132"/>
       <c r="M75" s="118"/>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="127"/>
       <c r="B76" s="127"/>
       <c r="C76" s="127"/>
@@ -4403,7 +4468,7 @@
       <c r="L76" s="132"/>
       <c r="M76" s="118"/>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="127" t="s">
         <v>62</v>
       </c>
@@ -4447,7 +4512,7 @@
       </c>
       <c r="M77" s="118"/>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="127" t="s">
         <v>63</v>
       </c>
@@ -4491,7 +4556,7 @@
       </c>
       <c r="M78" s="118"/>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="127" t="s">
         <v>64</v>
       </c>
@@ -4534,7 +4599,7 @@
       </c>
       <c r="M79" s="118"/>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="127" t="s">
         <v>65</v>
       </c>
@@ -4578,7 +4643,7 @@
       </c>
       <c r="M80" s="118"/>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="127" t="s">
         <v>66</v>
       </c>
@@ -4622,7 +4687,7 @@
       </c>
       <c r="M81" s="118"/>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="139"/>
       <c r="B82" s="139"/>
       <c r="C82" s="139"/>
@@ -4637,8 +4702,7 @@
       <c r="L82" s="139"/>
       <c r="M82" s="140"/>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="s">
         <v>39</v>
       </c>
@@ -4656,7 +4720,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G85" s="16" t="s">
         <v>41</v>
       </c>
@@ -4665,8 +4729,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -4675,7 +4738,7 @@
       <c r="G87" s="45"/>
       <c r="H87" s="141"/>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
@@ -4684,9 +4747,7 @@
       <c r="G88" s="45"/>
       <c r="H88" s="46"/>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="95"/>
       <c r="B91" s="95"/>
       <c r="C91" s="95"/>
@@ -4698,7 +4759,7 @@
       </c>
       <c r="H91" s="95"/>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="96" t="s">
         <v>68</v>
       </c>
@@ -4716,7 +4777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="24" t="s">
         <v>71</v>
       </c>
@@ -4732,7 +4793,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="24" t="s">
         <v>72</v>
       </c>
@@ -4748,7 +4809,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="24" t="s">
         <v>73</v>
       </c>
@@ -4764,7 +4825,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="24" t="s">
         <v>74</v>
       </c>
@@ -4780,7 +4841,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>75</v>
       </c>
@@ -4794,7 +4855,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>76</v>
       </c>
@@ -4808,7 +4869,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="24" t="s">
         <v>77</v>
       </c>
@@ -4824,7 +4885,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>78</v>
       </c>
@@ -4838,7 +4899,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>79</v>
       </c>
@@ -4852,7 +4913,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="24" t="s">
         <v>80</v>
       </c>
@@ -4868,7 +4929,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>81</v>
       </c>
@@ -4882,7 +4943,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>82</v>
       </c>
@@ -4896,7 +4957,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>83</v>
       </c>
@@ -4910,7 +4971,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="24" t="s">
         <v>84</v>
       </c>
@@ -4926,7 +4987,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>85</v>
       </c>
@@ -4940,7 +5001,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>86</v>
       </c>
@@ -4954,7 +5015,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>87</v>
       </c>
@@ -4968,7 +5029,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="24" t="s">
         <v>88</v>
       </c>
@@ -4984,7 +5045,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="24" t="s">
         <v>89</v>
       </c>
@@ -5001,11 +5062,11 @@
       </c>
     </row>
     <row r="113" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="156" t="s">
+      <c r="A113" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="B113" s="157"/>
-      <c r="C113" s="158"/>
+      <c r="B113" s="152"/>
+      <c r="C113" s="153"/>
       <c r="D113" s="122">
         <f>IF(D114="OMIT",D114,1-(D114/INSIZE)^2)</f>
         <v>-0.38062500000000021</v>
@@ -5058,11 +5119,11 @@
       <c r="W113" s="24"/>
     </row>
     <row r="114" spans="1:23" ht="12.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="166" t="s">
+      <c r="A114" s="154" t="s">
         <v>24</v>
       </c>
-      <c r="B114" s="167"/>
-      <c r="C114" s="168"/>
+      <c r="B114" s="155"/>
+      <c r="C114" s="156"/>
       <c r="D114" s="142">
         <v>4.7</v>
       </c>
@@ -5091,11 +5152,11 @@
       <c r="M114" s="126"/>
     </row>
     <row r="116" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="156" t="s">
+      <c r="A116" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="B116" s="157"/>
-      <c r="C116" s="158"/>
+      <c r="B116" s="152"/>
+      <c r="C116" s="153"/>
       <c r="D116" s="122">
         <f>IF(D117="OMIT",D117,1-(D117/INSIZE)^2)</f>
         <v>-3.7088999999999999</v>
@@ -5148,11 +5209,11 @@
       <c r="W116" s="24"/>
     </row>
     <row r="117" spans="1:23" ht="12.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="166" t="s">
+      <c r="A117" s="154" t="s">
         <v>24</v>
       </c>
-      <c r="B117" s="167"/>
-      <c r="C117" s="168"/>
+      <c r="B117" s="155"/>
+      <c r="C117" s="156"/>
       <c r="D117" s="142">
         <v>8.68</v>
       </c>
@@ -5182,22 +5243,22 @@
     </row>
     <row r="121" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A122" s="164">
+      <c r="A122" s="149">
         <v>8.5500000000000007</v>
       </c>
-      <c r="B122" s="164">
+      <c r="B122" s="149">
         <v>7.55</v>
       </c>
-      <c r="C122" s="164">
+      <c r="C122" s="149">
         <v>6.7</v>
       </c>
-      <c r="D122" s="164">
+      <c r="D122" s="149">
         <v>6</v>
       </c>
-      <c r="E122" s="164">
+      <c r="E122" s="149">
         <v>5.4</v>
       </c>
-      <c r="F122" s="164">
+      <c r="F122" s="149">
         <v>4.9000000000000004</v>
       </c>
       <c r="G122" s="145">
@@ -5205,12 +5266,12 @@
       </c>
     </row>
     <row r="123" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="165"/>
-      <c r="B123" s="165"/>
-      <c r="C123" s="165"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
-      <c r="F123" s="165"/>
+      <c r="A123" s="150"/>
+      <c r="B123" s="150"/>
+      <c r="C123" s="150"/>
+      <c r="D123" s="150"/>
+      <c r="E123" s="150"/>
+      <c r="F123" s="150"/>
       <c r="G123" s="146">
         <v>-4.38</v>
       </c>
@@ -5225,6 +5286,13 @@
     </scenario>
   </scenarios>
   <mergeCells count="17">
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:C63"/>
     <mergeCell ref="D122:D123"/>
     <mergeCell ref="E122:E123"/>
     <mergeCell ref="F122:F123"/>
@@ -5235,13 +5303,6 @@
     <mergeCell ref="A122:A123"/>
     <mergeCell ref="B122:B123"/>
     <mergeCell ref="C122:C123"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:C63"/>
   </mergeCells>
   <conditionalFormatting sqref="D24">
     <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="lessThan">
@@ -5343,7 +5404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>